<commit_message>
classes added to Utility package: - Constants - Excel - ImpWait - Links
</commit_message>
<xml_diff>
--- a/src/Data/Registration.xlsx
+++ b/src/Data/Registration.xlsx
@@ -3,20 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_projects\AutomationPractice\AutomationPracticeTest\src\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14550" windowHeight="5985"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="83">
   <si>
     <t>Test ID</t>
   </si>
@@ -279,7 +279,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -339,7 +338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -352,6 +351,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -635,21 +637,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="O5" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2:W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="20" max="21" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="54.85546875" collapsed="true"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.42578125" customWidth="1" collapsed="1"/>
+    <col min="20" max="21" width="10.42578125" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="54.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -762,11 +764,11 @@
         <v>30</v>
       </c>
       <c r="V2" s="2"/>
-      <c r="W2" s="2" t="s">
+      <c r="W2" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -811,7 +813,7 @@
       </c>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
-      <c r="W3" s="2" t="s">
+      <c r="W3" s="6" t="s">
         <v>74</v>
       </c>
     </row>
@@ -860,7 +862,7 @@
         <v>42</v>
       </c>
       <c r="V4" s="2"/>
-      <c r="W4" s="2" t="s">
+      <c r="W4" s="6" t="s">
         <v>75</v>
       </c>
     </row>
@@ -909,11 +911,11 @@
         <v>43</v>
       </c>
       <c r="V5" s="2"/>
-      <c r="W5" s="2" t="s">
+      <c r="W5" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>61</v>
       </c>
@@ -960,7 +962,7 @@
         <v>47</v>
       </c>
       <c r="V6" s="2"/>
-      <c r="W6" s="2" t="s">
+      <c r="W6" s="6" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1011,11 +1013,11 @@
         <v>51</v>
       </c>
       <c r="V7" s="2"/>
-      <c r="W7" s="2" t="s">
+      <c r="W7" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>65</v>
       </c>
@@ -1062,11 +1064,11 @@
         <v>54</v>
       </c>
       <c r="V8" s="2"/>
-      <c r="W8" s="2" t="s">
+      <c r="W8" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>63</v>
       </c>
@@ -1113,11 +1115,11 @@
         <v>57</v>
       </c>
       <c r="V9" s="2"/>
-      <c r="W9" s="2" t="s">
+      <c r="W9" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>64</v>
       </c>
@@ -1162,11 +1164,11 @@
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
-      <c r="W10" s="2" t="s">
+      <c r="W10" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>66</v>
       </c>
@@ -1205,7 +1207,7 @@
         <v>30</v>
       </c>
       <c r="V11" s="2"/>
-      <c r="W11" s="2" t="s">
+      <c r="W11" s="6" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>